<commit_message>
Inclusión de campos y validaciones paso 1
</commit_message>
<xml_diff>
--- a/website/Formatos/FormatoTDC_P1.xlsx
+++ b/website/Formatos/FormatoTDC_P1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>tipo_doc</t>
   </si>
@@ -36,19 +36,31 @@
   </si>
   <si>
     <t>proceso</t>
+  </si>
+  <si>
+    <t>fecha_venta</t>
+  </si>
+  <si>
+    <t>2022-03-21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -59,7 +71,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -67,12 +79,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0D7E5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD0D7E5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD0D7E5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0D7E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,15 +383,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.42578125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,8 +407,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -388,8 +424,11 @@
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -401,6 +440,9 @@
       </c>
       <c r="D3">
         <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>